<commit_message>
Finished first version of Use Cases and crosstable with functional requirements
</commit_message>
<xml_diff>
--- a/FR-UC crosstable.xlsx
+++ b/FR-UC crosstable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruudd\source\repos\dota2rpg\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C6F8384F-6989-49B9-8A72-609AD6E0253C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>FR-01</t>
   </si>
@@ -125,12 +126,6 @@
     <t>Q-10.1</t>
   </si>
   <si>
-    <t>R-10.2</t>
-  </si>
-  <si>
-    <t>Q-10.3</t>
-  </si>
-  <si>
     <t>R-11.1</t>
   </si>
   <si>
@@ -234,12 +229,15 @@
   </si>
   <si>
     <t>Q-03.5</t>
+  </si>
+  <si>
+    <t>Q-10.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -580,11 +578,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB89"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AB88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Y52" sqref="Y52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,73 +593,73 @@
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
@@ -673,13 +671,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -711,7 +709,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -745,7 +743,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -779,7 +777,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -812,7 +810,7 @@
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -845,7 +843,7 @@
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -879,13 +877,13 @@
       <c r="B8" s="8"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -916,7 +914,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -944,16 +942,16 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -979,13 +977,13 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -1012,14 +1010,14 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -1045,15 +1043,15 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -1088,7 +1086,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -1121,7 +1119,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1154,7 +1152,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1187,7 +1185,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1221,7 +1219,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -1254,7 +1252,7 @@
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -1288,7 +1286,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -1321,7 +1319,9 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="J21" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
@@ -1352,7 +1352,9 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
+      <c r="J22" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
@@ -1383,7 +1385,9 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
+      <c r="J23" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
@@ -1415,7 +1419,9 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="K24" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
@@ -1446,7 +1452,9 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="K25" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
@@ -1477,7 +1485,9 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
+      <c r="K26" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
@@ -1509,7 +1519,9 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
+      <c r="L27" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
@@ -1540,7 +1552,9 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
+      <c r="L28" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
@@ -1572,7 +1586,9 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
+      <c r="M29" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
@@ -1603,7 +1619,9 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
+      <c r="M30" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
@@ -1634,7 +1652,9 @@
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
+      <c r="M31" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
@@ -1666,8 +1686,12 @@
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
+      <c r="N32" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
@@ -1697,7 +1721,9 @@
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
+      <c r="N33" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
@@ -1714,7 +1740,7 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="6"/>
@@ -1729,7 +1755,9 @@
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
+      <c r="O34" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
@@ -1744,8 +1772,8 @@
       <c r="AA34" s="6"/>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>34</v>
+      <c r="A35" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="6"/>
@@ -1761,7 +1789,9 @@
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
+      <c r="P35" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
       <c r="S35" s="6"/>
@@ -1775,8 +1805,8 @@
       <c r="AA35" s="6"/>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>10</v>
+      <c r="A36" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="6"/>
@@ -1792,7 +1822,9 @@
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
+      <c r="P36" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="Q36" s="6"/>
       <c r="R36" s="6"/>
       <c r="S36" s="6"/>
@@ -1806,8 +1838,8 @@
       <c r="AA36" s="6"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>35</v>
+      <c r="A37" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="6"/>
@@ -1824,7 +1856,9 @@
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
+      <c r="Q37" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="R37" s="6"/>
       <c r="S37" s="6"/>
       <c r="T37" s="6"/>
@@ -1837,8 +1871,8 @@
       <c r="AA37" s="6"/>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>11</v>
+      <c r="A38" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="6"/>
@@ -1855,7 +1889,9 @@
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
+      <c r="Q38" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="R38" s="6"/>
       <c r="S38" s="6"/>
       <c r="T38" s="6"/>
@@ -1868,8 +1904,8 @@
       <c r="AA38" s="6"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>36</v>
+      <c r="A39" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="6"/>
@@ -1887,7 +1923,9 @@
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
+      <c r="R39" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="S39" s="6"/>
       <c r="T39" s="6"/>
       <c r="U39" s="6"/>
@@ -1899,8 +1937,8 @@
       <c r="AA39" s="6"/>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>12</v>
+      <c r="A40" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="6"/>
@@ -1918,7 +1956,9 @@
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
+      <c r="R40" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="S40" s="6"/>
       <c r="T40" s="6"/>
       <c r="U40" s="6"/>
@@ -1930,8 +1970,8 @@
       <c r="AA40" s="6"/>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>37</v>
+      <c r="A41" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="6"/>
@@ -1950,7 +1990,9 @@
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
       <c r="R41" s="6"/>
-      <c r="S41" s="6"/>
+      <c r="S41" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="T41" s="6"/>
       <c r="U41" s="6"/>
       <c r="V41" s="6"/>
@@ -1961,8 +2003,8 @@
       <c r="AA41" s="6"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>13</v>
+      <c r="A42" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="6"/>
@@ -1981,7 +2023,9 @@
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
-      <c r="S42" s="6"/>
+      <c r="S42" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
       <c r="V42" s="6"/>
@@ -1992,8 +2036,8 @@
       <c r="AA42" s="6"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>38</v>
+      <c r="A43" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -2013,7 +2057,9 @@
       <c r="Q43" s="6"/>
       <c r="R43" s="6"/>
       <c r="S43" s="6"/>
-      <c r="T43" s="6"/>
+      <c r="T43" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="U43" s="6"/>
       <c r="V43" s="6"/>
       <c r="W43" s="6"/>
@@ -2023,8 +2069,8 @@
       <c r="AA43" s="6"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>14</v>
+      <c r="A44" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -2044,9 +2090,13 @@
       <c r="Q44" s="6"/>
       <c r="R44" s="6"/>
       <c r="S44" s="6"/>
-      <c r="T44" s="6"/>
+      <c r="T44" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="U44" s="6"/>
-      <c r="V44" s="6"/>
+      <c r="V44" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="W44" s="6"/>
       <c r="X44" s="6"/>
       <c r="Y44" s="6"/>
@@ -2055,7 +2105,7 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -2075,8 +2125,12 @@
       <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
       <c r="S45" s="6"/>
-      <c r="T45" s="6"/>
-      <c r="U45" s="6"/>
+      <c r="T45" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U45" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="V45" s="6"/>
       <c r="W45" s="6"/>
       <c r="X45" s="6"/>
@@ -2086,7 +2140,7 @@
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -2106,8 +2160,12 @@
       <c r="Q46" s="6"/>
       <c r="R46" s="6"/>
       <c r="S46" s="6"/>
-      <c r="T46" s="6"/>
-      <c r="U46" s="6"/>
+      <c r="T46" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U46" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="V46" s="6"/>
       <c r="W46" s="6"/>
       <c r="X46" s="6"/>
@@ -2116,20 +2174,21 @@
       <c r="AA46" s="6"/>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V47" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A48" s="4"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
+      <c r="A49" s="1"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
+      <c r="A50" s="4"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
@@ -2141,10 +2200,10 @@
       <c r="A53" s="4"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
+      <c r="A54" s="1"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
+      <c r="A55" s="4"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
@@ -2153,19 +2212,19 @@
       <c r="A57" s="4"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
+      <c r="A58" s="1"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
+      <c r="A59" s="4"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
+      <c r="A61" s="1"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
+      <c r="A62" s="4"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
@@ -2244,9 +2303,6 @@
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>